<commit_message>
cbo nipa comparison and flow chart updates
</commit_message>
<xml_diff>
--- a/CBO NIPA comparison.xlsx
+++ b/CBO NIPA comparison.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D4518-0165-4F30-A74D-F749A6C63266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1582B3-B599-48EF-95A0-DA1B7D15414F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4596,8 +4596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9589D34-1559-4E02-B9F6-794E0F2B6B2D}">
   <dimension ref="A2:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="69" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="69" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6265,13 +6265,13 @@
         <v>1053</v>
       </c>
       <c r="L31" s="83">
-        <v>1072</v>
+        <v>1055</v>
       </c>
       <c r="M31" s="83">
-        <v>911</v>
+        <v>863</v>
       </c>
       <c r="N31" s="91">
-        <v>965</v>
+        <v>880</v>
       </c>
       <c r="O31" s="82"/>
     </row>
@@ -9256,53 +9256,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver xmlns="">
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver xmlns="">
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver xmlns="">
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver xmlns="">
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a">45RU2JKQZF2C-997389622-57</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a">
+      <Url>https://cbogov.sharepoint.com/sites/cbolife/resources/editing-publishing/_layouts/15/DocIdRedir.aspx?ID=45RU2JKQZF2C-997389622-57</Url>
+      <Description>45RU2JKQZF2C-997389622-57</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9513,17 +9477,53 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a">45RU2JKQZF2C-997389622-57</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a">
-      <Url>https://cbogov.sharepoint.com/sites/cbolife/resources/editing-publishing/_layouts/15/DocIdRedir.aspx?ID=45RU2JKQZF2C-997389622-57</Url>
-      <Description>45RU2JKQZF2C-997389622-57</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver xmlns="">
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver xmlns="">
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver xmlns="">
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver xmlns="">
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9536,10 +9536,12 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{310CEC0E-29D0-4545-A3A0-AD5C4D8B850A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A04B03F-C5FA-4EBD-8DCF-4A46F3164370}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9565,12 +9567,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A04B03F-C5FA-4EBD-8DCF-4A46F3164370}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{310CEC0E-29D0-4545-A3A0-AD5C4D8B850A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="76cf5f1b-7b29-42e3-a6af-ab0bb9e3e73a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>